<commit_message>
hefte sonu gunluk hesabat
</commit_message>
<xml_diff>
--- a/static/data/quizz.xlsx
+++ b/static/data/quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DERS\Archive\web\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C597447-A063-45E4-AB0B-047914097D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FDC2E7-E5C4-48D7-A7C3-ED21206A1AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,7 +820,7 @@
   <dimension ref="A1:BE24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,7 +2545,7 @@
         <v>73</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>

</xml_diff>